<commit_message>
fixing typo in patient IDs
</commit_message>
<xml_diff>
--- a/python/resources/Patients_Catalog.xlsx
+++ b/python/resources/Patients_Catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\BioTAU\Huntington\python\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E3E352-BEEB-4447-9786-FCC4F687E76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DE6A58-821D-49CC-AD91-655E983A10AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="82">
   <si>
     <t>Cell_Type</t>
   </si>
@@ -45,9 +45,6 @@
     <t>CAP_Score</t>
   </si>
   <si>
-    <t xml:space="preserve"> Disease_Severity</t>
-  </si>
-  <si>
     <t>HC</t>
   </si>
   <si>
@@ -63,18 +60,12 @@
     <t>AG16146</t>
   </si>
   <si>
-    <t>HD</t>
-  </si>
-  <si>
     <t>GM00305</t>
   </si>
   <si>
     <t>F</t>
   </si>
   <si>
-    <t xml:space="preserve"> Severe</t>
-  </si>
-  <si>
     <t>GM00726</t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t>GM04196</t>
   </si>
   <si>
-    <t xml:space="preserve"> Mild</t>
-  </si>
-  <si>
     <t>GM04200</t>
   </si>
   <si>
@@ -117,9 +105,6 @@
     <t>GM04689</t>
   </si>
   <si>
-    <t xml:space="preserve"> Premanifest</t>
-  </si>
-  <si>
     <t>GM04691</t>
   </si>
   <si>
@@ -138,9 +123,6 @@
     <t>GM04719</t>
   </si>
   <si>
-    <t>Premanifest</t>
-  </si>
-  <si>
     <t>GM04721</t>
   </si>
   <si>
@@ -180,9 +162,6 @@
     <t>HGPS</t>
   </si>
   <si>
-    <t>HGADFN0013</t>
-  </si>
-  <si>
     <t>HGADFN0122</t>
   </si>
   <si>
@@ -277,6 +256,21 @@
   </si>
   <si>
     <t>NA7525</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>HGADFN0143</t>
+  </si>
+  <si>
+    <t>HD_Severe</t>
+  </si>
+  <si>
+    <t>HD_Mild</t>
+  </si>
+  <si>
+    <t>HD_Premanifest</t>
   </si>
 </sst>
 </file>
@@ -571,25 +565,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G997"/>
+  <dimension ref="A1:F997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="9.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="26" width="8.6640625" customWidth="1"/>
+    <col min="7" max="25" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -608,68 +601,59 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="6">
         <v>1.5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="7">
         <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="7">
         <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="7">
         <v>45</v>
@@ -677,91 +661,79 @@
       <c r="F4" s="6">
         <v>129.4299</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C5" s="7">
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C6" s="7">
         <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" s="7">
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" s="7">
         <v>55</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="7">
         <v>44</v>
@@ -769,22 +741,19 @@
       <c r="F8" s="6">
         <v>118.64409999999999</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="7">
         <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="7">
         <v>46</v>
@@ -792,22 +761,19 @@
       <c r="F9" s="6">
         <v>140.5239</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="7">
         <v>51</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" s="7">
         <v>44</v>
@@ -815,22 +781,19 @@
       <c r="F10" s="6">
         <v>110.0154</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>12</v>
+    </row>
+    <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C11" s="7">
         <v>53</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="7">
         <v>46</v>
@@ -838,22 +801,19 @@
       <c r="F11" s="6">
         <v>130.6626</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C12" s="7">
         <v>50</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E12" s="7">
         <v>43</v>
@@ -861,22 +821,19 @@
       <c r="F12" s="6">
         <v>100.1541</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="7">
         <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="7">
         <v>51</v>
@@ -884,22 +841,19 @@
       <c r="F13" s="6">
         <v>129.4299</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
+    </row>
+    <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C14" s="7">
         <v>43</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="7">
         <v>49</v>
@@ -907,22 +861,19 @@
       <c r="F14" s="6">
         <v>125.886</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>12</v>
+    </row>
+    <row r="15" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C15" s="7">
         <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="7">
         <v>45</v>
@@ -930,22 +881,19 @@
       <c r="F15" s="6">
         <v>131.74109999999999</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C16" s="7">
         <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E16" s="7">
         <v>50</v>
@@ -953,22 +901,19 @@
       <c r="F16" s="6">
         <v>114.02160000000001</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C17" s="7">
         <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17" s="7">
         <v>45</v>
@@ -976,22 +921,19 @@
       <c r="F17" s="6">
         <v>69.337440000000001</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C18" s="7">
         <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="7">
         <v>54</v>
@@ -999,22 +941,19 @@
       <c r="F18" s="6">
         <v>114.6379</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C19" s="7">
         <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="7">
         <v>45</v>
@@ -1022,22 +961,19 @@
       <c r="F19" s="6">
         <v>76.271190000000004</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C20" s="7">
         <v>38</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20" s="7">
         <v>49</v>
@@ -1045,22 +981,19 @@
       <c r="F20" s="6">
         <v>111.24809999999999</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C21" s="7">
         <v>40</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" s="7">
         <v>48</v>
@@ -1068,22 +1001,19 @@
       <c r="F21" s="6">
         <v>110.93989999999999</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>12</v>
+    </row>
+    <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C22" s="7">
         <v>44</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E22" s="7">
         <v>41</v>
@@ -1091,22 +1021,19 @@
       <c r="F22" s="6">
         <v>74.576269999999994</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>12</v>
+    </row>
+    <row r="23" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C23" s="7">
         <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E23" s="7">
         <v>44</v>
@@ -1114,22 +1041,19 @@
       <c r="F23" s="6">
         <v>84.129429999999999</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C24" s="7">
         <v>37</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E24" s="7">
         <v>46</v>
@@ -1137,22 +1061,19 @@
       <c r="F24" s="6">
         <v>91.217259999999996</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>12</v>
+    </row>
+    <row r="25" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C25" s="7">
         <v>43</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E25" s="7">
         <v>46</v>
@@ -1160,22 +1081,19 @@
       <c r="F25" s="6">
         <v>106.00920000000001</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C26" s="7">
         <v>47</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="7">
         <v>43</v>
@@ -1183,22 +1101,19 @@
       <c r="F26" s="6">
         <v>94.144840000000002</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C27" s="7">
         <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="7">
         <v>50</v>
@@ -1206,22 +1121,19 @@
       <c r="F27" s="6">
         <v>126.34820000000001</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C28" s="7">
         <v>48</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="7">
         <v>43</v>
@@ -1229,22 +1141,19 @@
       <c r="F28" s="6">
         <v>96.147919999999999</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C29" s="7">
         <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="7">
         <v>47</v>
@@ -1252,22 +1161,19 @@
       <c r="F29" s="6">
         <v>60.24653</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C30" s="7">
         <v>31</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" s="7">
         <v>46</v>
@@ -1275,22 +1181,19 @@
       <c r="F30" s="6">
         <v>76.425269999999998</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
-        <v>12</v>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C31" s="7">
         <v>28</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E31" s="7">
         <v>54</v>
@@ -1298,22 +1201,19 @@
       <c r="F31" s="6">
         <v>103.54389999999999</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C32" s="7">
         <v>48</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E32" s="7">
         <v>45</v>
@@ -1321,22 +1221,19 @@
       <c r="F32" s="6">
         <v>110.93989999999999</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>12</v>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C33" s="7">
         <v>60</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E33" s="7">
         <v>45</v>
@@ -1344,22 +1241,19 @@
       <c r="F33" s="6">
         <v>138.67490000000001</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>12</v>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C34" s="7">
         <v>56</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E34" s="7">
         <v>45</v>
@@ -1367,848 +1261,758 @@
       <c r="F34" s="6">
         <v>129.4299</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C35" s="7">
         <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="C36" s="7">
         <v>0</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C37" s="7">
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C38" s="6">
         <v>3.75</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C39" s="6">
         <v>8.5</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C40" s="6">
         <v>2.25</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C41" s="6">
         <v>1.25</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C42" s="7">
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C43" s="7">
         <v>48</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C44" s="7">
         <v>2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C45" s="7">
         <v>42</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C46" s="7">
         <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C47" s="7">
         <v>68</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C48" s="7">
         <v>61</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C49" s="7">
         <v>51</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C50" s="7">
         <v>62</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C51" s="7">
         <v>56</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C52" s="7">
         <v>53</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C53" s="7">
         <v>68</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C54" s="7">
         <v>49</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C55" s="7">
         <v>48</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C56" s="7">
         <v>40</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G56" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C57" s="7">
         <v>50</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C58" s="7">
         <v>51</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C59" s="7">
         <v>46</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C60" s="7">
         <v>50</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C61" s="7">
         <v>48</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C62" s="7">
         <v>52</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C63" s="7">
         <v>61</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C64" s="7">
         <v>56</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C65" s="7">
         <v>50</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C66" s="7">
         <v>62</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C67" s="7">
         <v>43</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C68" s="7">
         <v>4</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="8"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="10"/>
-    </row>
-    <row r="70" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C69" s="8">
+        <v>0</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C70" s="8"/>
       <c r="E70" s="9"/>
       <c r="F70" s="10"/>
     </row>
-    <row r="71" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C71" s="8"/>
       <c r="E71" s="9"/>
       <c r="F71" s="10"/>
     </row>
-    <row r="72" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C72" s="8"/>
       <c r="E72" s="9"/>
       <c r="F72" s="10"/>
     </row>
-    <row r="73" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C73" s="8"/>
       <c r="E73" s="9"/>
       <c r="F73" s="10"/>
     </row>
-    <row r="74" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C74" s="8"/>
       <c r="E74" s="9"/>
       <c r="F74" s="10"/>
     </row>
-    <row r="75" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C75" s="8"/>
       <c r="E75" s="9"/>
       <c r="F75" s="10"/>
     </row>
-    <row r="76" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C76" s="8"/>
       <c r="E76" s="9"/>
       <c r="F76" s="10"/>
     </row>
-    <row r="77" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C77" s="8"/>
       <c r="E77" s="9"/>
       <c r="F77" s="10"/>
     </row>
-    <row r="78" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C78" s="8"/>
       <c r="E78" s="9"/>
       <c r="F78" s="10"/>
     </row>
-    <row r="79" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C79" s="8"/>
       <c r="E79" s="9"/>
       <c r="F79" s="10"/>
     </row>
-    <row r="80" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C80" s="8"/>
       <c r="E80" s="9"/>
       <c r="F80" s="10"/>

</xml_diff>

<commit_message>
change status "HC" to "Healthy"
</commit_message>
<xml_diff>
--- a/python/resources/Patients_Catalog.xlsx
+++ b/python/resources/Patients_Catalog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\BioTAU\Huntington\python\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA84E2FD-E26B-4324-88E4-707FB73BE441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4B6442-CD47-414B-B553-26AFF11E1325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12060" yWindow="336" windowWidth="10980" windowHeight="12024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>CAP_Score</t>
   </si>
   <si>
-    <t>HC</t>
-  </si>
-  <si>
     <t>AG0015</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>Disease_Status</t>
+  </si>
+  <si>
+    <t>Healthy</t>
   </si>
 </sst>
 </file>
@@ -568,7 +568,7 @@
   <dimension ref="A1:F997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -584,7 +584,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -604,56 +604,56 @@
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C2" s="6">
         <v>1.5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="7">
         <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="7">
         <v>56</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="7">
         <v>45</v>
@@ -664,76 +664,76 @@
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="7">
         <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="7">
         <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="7">
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="7">
         <v>55</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="7">
         <v>44</v>
@@ -744,16 +744,16 @@
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="7">
         <v>57</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="7">
         <v>46</v>
@@ -764,16 +764,16 @@
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7">
         <v>51</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="7">
         <v>44</v>
@@ -784,16 +784,16 @@
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="7">
         <v>53</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="7">
         <v>46</v>
@@ -804,16 +804,16 @@
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="7">
         <v>50</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12" s="7">
         <v>43</v>
@@ -824,16 +824,16 @@
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="7">
         <v>40</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="7">
         <v>51</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" s="7">
         <v>43</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="7">
         <v>49</v>
@@ -864,16 +864,16 @@
     </row>
     <row r="15" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="7">
         <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="7">
         <v>45</v>
@@ -884,16 +884,16 @@
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" s="7">
         <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="7">
         <v>50</v>
@@ -904,16 +904,16 @@
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" s="7">
         <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E17" s="7">
         <v>45</v>
@@ -924,16 +924,16 @@
     </row>
     <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="7">
         <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="7">
         <v>54</v>
@@ -944,16 +944,16 @@
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="7">
         <v>33</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="7">
         <v>45</v>
@@ -964,16 +964,16 @@
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="7">
         <v>38</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E20" s="7">
         <v>49</v>
@@ -984,16 +984,16 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="7">
         <v>40</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="7">
         <v>48</v>
@@ -1004,16 +1004,16 @@
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="7">
         <v>44</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E22" s="7">
         <v>41</v>
@@ -1024,16 +1024,16 @@
     </row>
     <row r="23" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="7">
         <v>39</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E23" s="7">
         <v>44</v>
@@ -1044,16 +1044,16 @@
     </row>
     <row r="24" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="7">
         <v>37</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E24" s="7">
         <v>46</v>
@@ -1064,16 +1064,16 @@
     </row>
     <row r="25" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="7">
         <v>43</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E25" s="7">
         <v>46</v>
@@ -1084,16 +1084,16 @@
     </row>
     <row r="26" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="7">
         <v>47</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" s="7">
         <v>43</v>
@@ -1104,16 +1104,16 @@
     </row>
     <row r="27" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="7">
         <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" s="7">
         <v>50</v>
@@ -1124,16 +1124,16 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="7">
         <v>48</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28" s="7">
         <v>43</v>
@@ -1144,16 +1144,16 @@
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29" s="7">
         <v>23</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29" s="7">
         <v>47</v>
@@ -1164,16 +1164,16 @@
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="7">
         <v>31</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30" s="7">
         <v>46</v>
@@ -1184,16 +1184,16 @@
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="7">
         <v>28</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E31" s="7">
         <v>54</v>
@@ -1204,16 +1204,16 @@
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" s="7">
         <v>48</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E32" s="7">
         <v>45</v>
@@ -1224,16 +1224,16 @@
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="7">
         <v>60</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33" s="7">
         <v>45</v>
@@ -1244,16 +1244,16 @@
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" s="7">
         <v>56</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E34" s="7">
         <v>45</v>
@@ -1264,702 +1264,702 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" s="7">
         <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="7">
         <v>0</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C37" s="7">
         <v>5</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" s="6">
         <v>3.75</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" s="6">
         <v>8.5</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" s="6">
         <v>2.25</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" s="6">
         <v>1.25</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="7">
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>5</v>
+      <c r="A43" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" s="7">
         <v>48</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="7">
         <v>2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>5</v>
+      <c r="A45" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" s="7">
         <v>42</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>5</v>
+      <c r="A46" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C46" s="7">
         <v>55</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>5</v>
+      <c r="A47" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C47" s="7">
         <v>68</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>5</v>
+      <c r="A48" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="7">
         <v>61</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>5</v>
+      <c r="A49" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="7">
         <v>51</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>5</v>
+      <c r="A50" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C50" s="7">
         <v>62</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>5</v>
+      <c r="A51" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C51" s="7">
         <v>56</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C52" s="7">
         <v>53</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
-        <v>5</v>
+      <c r="A53" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53" s="7">
         <v>68</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>5</v>
+      <c r="A54" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="7">
         <v>49</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
-        <v>5</v>
+      <c r="A55" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="7">
         <v>48</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>5</v>
+      <c r="A56" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C56" s="7">
         <v>40</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C57" s="7">
         <v>50</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" s="7">
         <v>51</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
-        <v>5</v>
+      <c r="A59" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" s="7">
         <v>46</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>5</v>
+      <c r="A60" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60" s="7">
         <v>50</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>5</v>
+      <c r="A61" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" s="7">
         <v>48</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" s="7">
         <v>52</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C63" s="7">
         <v>61</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C64" s="7">
         <v>56</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>5</v>
+      <c r="A65" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C65" s="7">
         <v>50</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C66" s="7">
         <v>62</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>5</v>
+      <c r="A67" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67" s="7">
         <v>43</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C68" s="7">
         <v>4</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="3" t="s">
-        <v>5</v>
+      <c r="A69" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C69" s="8">
         <v>0</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>